<commit_message>
Feat: update e2e tests :sparkles: (#84)
</commit_message>
<xml_diff>
--- a/cypress/fixtures/TEMPLATE_CHATBOT-WARNING.xlsx
+++ b/cypress/fixtures/TEMPLATE_CHATBOT-WARNING.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22624"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23231"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\laine\Documents\beta.gouv\fabrique-chatbot-front\cypress\fixtures\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\laine\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC522263-8186-465F-BD23-699B39E44CBF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{040B64AC-1874-4DE3-AF13-05211D72B26A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="15796" xr2:uid="{585389C5-6A76-482F-A969-368084FBEB95}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="52">
   <si>
     <t>ID</t>
   </si>
@@ -180,6 +180,15 @@
   </si>
   <si>
     <t>phrase_hors_sujet</t>
+  </si>
+  <si>
+    <t>phrase_feedback</t>
+  </si>
+  <si>
+    <t>Bonjour, cet ID correspond au message envoyé quand un utilisateur donne son avis sur une réponse.</t>
+  </si>
+  <si>
+    <t>Phrase feedback.; J'ai laissé mon avis !</t>
   </si>
 </sst>
 </file>
@@ -574,11 +583,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{63FF1A2E-52F7-4FFB-A61E-6AFA2252F37F}">
-  <dimension ref="A1:G20"/>
+  <dimension ref="A1:G21"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="107" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="C3" sqref="C3"/>
+      <selection pane="topRight" activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -644,35 +653,38 @@
         <v>46</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:7" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A5" t="s">
-        <v>25</v>
-      </c>
-      <c r="C5" t="s">
-        <v>26</v>
+        <v>49</v>
       </c>
       <c r="D5" t="s">
         <v>3</v>
       </c>
       <c r="E5" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="G5" s="7" t="s">
-        <v>27</v>
+        <v>50</v>
+      </c>
+      <c r="G5" t="s">
+        <v>51</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A6" t="s">
         <v>25</v>
       </c>
+      <c r="C6" t="s">
+        <v>26</v>
+      </c>
       <c r="D6" t="s">
         <v>3</v>
       </c>
       <c r="E6" s="4" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" ht="28.5" x14ac:dyDescent="0.45">
+        <v>12</v>
+      </c>
+      <c r="G6" s="7" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A7" t="s">
         <v>25</v>
       </c>
@@ -680,99 +692,99 @@
         <v>3</v>
       </c>
       <c r="E7" s="4" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="A8" t="s">
+        <v>25</v>
+      </c>
+      <c r="D8" t="s">
+        <v>3</v>
+      </c>
+      <c r="E8" s="4" t="s">
         <v>10</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A8" t="s">
-        <v>13</v>
-      </c>
-      <c r="C8" t="s">
-        <v>14</v>
-      </c>
-      <c r="D8" t="s">
-        <v>3</v>
-      </c>
-      <c r="E8" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="G8" s="7" t="s">
-        <v>16</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A9" t="s">
         <v>13</v>
       </c>
+      <c r="C9" t="s">
+        <v>14</v>
+      </c>
       <c r="D9" t="s">
-        <v>8</v>
-      </c>
-      <c r="E9" s="5" t="s">
-        <v>15</v>
+        <v>3</v>
+      </c>
+      <c r="E9" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="G9" s="7" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A10" t="s">
-        <v>18</v>
-      </c>
-      <c r="C10" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="D10" t="s">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="E10" s="5" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A11" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="C11" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="D11" t="s">
         <v>3</v>
       </c>
-      <c r="E11" s="4" t="s">
-        <v>24</v>
+      <c r="E11" s="5" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A12" t="s">
         <v>21</v>
       </c>
+      <c r="C12" t="s">
+        <v>22</v>
+      </c>
       <c r="D12" t="s">
-        <v>9</v>
+        <v>3</v>
       </c>
       <c r="E12" s="4" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A13" t="s">
-        <v>28</v>
-      </c>
-      <c r="C13" t="s">
-        <v>29</v>
+        <v>21</v>
       </c>
       <c r="D13" t="s">
-        <v>3</v>
+        <v>9</v>
       </c>
       <c r="E13" s="4" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" ht="28.5" x14ac:dyDescent="0.45">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A14" t="s">
         <v>28</v>
       </c>
+      <c r="C14" t="s">
+        <v>29</v>
+      </c>
       <c r="D14" t="s">
         <v>3</v>
       </c>
       <c r="E14" s="4" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="15" spans="1:7" ht="28.5" x14ac:dyDescent="0.45">
@@ -783,7 +795,7 @@
         <v>3</v>
       </c>
       <c r="E15" s="4" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="16" spans="1:7" ht="28.5" x14ac:dyDescent="0.45">
@@ -791,75 +803,86 @@
         <v>28</v>
       </c>
       <c r="D16" t="s">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="E16" s="4" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="17" spans="1:5" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A17" t="s">
-        <v>34</v>
-      </c>
-      <c r="C17" t="s">
-        <v>43</v>
+        <v>28</v>
       </c>
       <c r="D17" t="s">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="E17" s="4" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
     </row>
     <row r="18" spans="1:5" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A18" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C18" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="D18" t="s">
         <v>3</v>
       </c>
       <c r="E18" s="4" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="19" spans="1:5" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A19" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C19" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="D19" t="s">
         <v>3</v>
       </c>
       <c r="E19" s="4" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.45">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A20" t="s">
         <v>36</v>
       </c>
+      <c r="C20" t="s">
+        <v>40</v>
+      </c>
       <c r="D20" t="s">
         <v>3</v>
       </c>
       <c r="E20" s="4" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A21" t="s">
+        <v>36</v>
+      </c>
+      <c r="D21" t="s">
+        <v>3</v>
+      </c>
+      <c r="E21" s="4" t="s">
         <v>41</v>
       </c>
     </row>
   </sheetData>
   <dataValidations count="2">
-    <dataValidation allowBlank="1" showInputMessage="1" sqref="B1 B6:B1048576" xr:uid="{2294A2A3-FB38-4AB2-86DB-236358F69018}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" sqref="B1 B7:B1048576" xr:uid="{2294A2A3-FB38-4AB2-86DB-236358F69018}"/>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D1048576" xr:uid="{2F3046D0-9243-4C0B-A990-964A502BF084}">
       <formula1>"Texte,Lien,Réponse à choix,Image"</formula1>
     </dataValidation>
   </dataValidations>
   <hyperlinks>
-    <hyperlink ref="E9" r:id="rId1" xr:uid="{285BDA86-05E1-4893-8CD7-0E0F567D7D4A}"/>
-    <hyperlink ref="E10" r:id="rId2" xr:uid="{17E4C6F7-A3EB-4B54-8DD2-FBF61164AD90}"/>
+    <hyperlink ref="E10" r:id="rId1" xr:uid="{285BDA86-05E1-4893-8CD7-0E0F567D7D4A}"/>
+    <hyperlink ref="E11" r:id="rId2" xr:uid="{17E4C6F7-A3EB-4B54-8DD2-FBF61164AD90}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId3"/>

</xml_diff>